<commit_message>
Market data. Num scenarios updated.
</commit_message>
<xml_diff>
--- a/data/CS3/Market Data/CS3_market_data_2025.xlsx
+++ b/data/CS3/Market Data/CS3_market_data_2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\CS3\Market Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B42CB4-4B71-410C-B499-C9C0E4B0E6BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD3B930-0CBA-45EC-804B-02B3026A7761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45105" yWindow="-9990" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -1325,7 +1325,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1338,19 +1338,19 @@
         <v>1</v>
       </c>
       <c r="B1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1">
-        <f>1/3</f>
-        <v>0.33333333333333331</v>
+        <f>1/$B$1</f>
+        <v>1</v>
       </c>
       <c r="D1" s="1">
-        <f>1/3</f>
-        <v>0.33333333333333331</v>
+        <f t="shared" ref="D1:E1" si="0">1/$B$1</f>
+        <v>1</v>
       </c>
       <c r="E1" s="1">
-        <f>1/3</f>
-        <v>0.33333333333333331</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>

</xml_diff>